<commit_message>
fully merged EV-Base Load modules
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,16 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mseduculiegebe-my.sharepoint.com/personal/noe_diffels_student_uliege_be/Documents/Ordi - Bureau/Ordi - ULG/Job - Load Shifting/ULG_Flex_Residential_Load/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_75FB7AE426D7D3644CBF663AB805D8CA4BC093CE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD6AB710-BE7C-49F9-829D-10A633053C7E}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="main"/>
-    <sheet r:id="rId2" sheetId="2" name="Liste_données"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="Liste_données" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -254,9 +273,6 @@
     <t xml:space="preserve">Type de flexibilité </t>
   </si>
   <si>
-    <r>
-      <t/>
-    </r>
     <r>
       <rPr>
         <b/>
@@ -375,9 +391,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +448,19 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -443,22 +471,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5983b0"/>
+        <fgColor rgb="FF5983B0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFb2b2b2"/>
+        <fgColor rgb="FFB2B2B2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFf2f2f2"/>
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -479,16 +507,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,89 +524,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -589,10 +609,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -630,71 +650,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -722,7 +742,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -745,11 +765,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -758,13 +778,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -774,7 +794,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -783,7 +803,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -792,7 +812,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -800,10 +820,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -868,441 +888,385 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="8" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="40.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="2.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="56.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.25">
-      <c r="A1" s="10"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="4"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17">
-        <v>2</v>
-      </c>
-      <c r="E4" s="18" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="14">
+        <v>30</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>42</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="19">
+      <c r="C5" s="13"/>
+      <c r="D5" s="16">
         <f>1/6</f>
-      </c>
-      <c r="E5" s="18" t="s">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>46</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17">
+      <c r="C6" s="13"/>
+      <c r="D6" s="14">
         <v>1</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="21">
+      <c r="C10" s="13"/>
+      <c r="D10" s="18">
         <v>1</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="18"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="21">
+      <c r="C11" s="13"/>
+      <c r="D11" s="18">
         <v>4</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="18"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="22" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="22" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="22" t="s">
+      <c r="C14" s="13"/>
+      <c r="D14" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="22" t="s">
+      <c r="C16" s="13"/>
+      <c r="D16" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="22" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="22" t="s">
+      <c r="C18" s="13"/>
+      <c r="D18" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="22" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="6"/>
-      <c r="B22" s="23" t="s">
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="214.19999999999996">
+    </row>
+    <row r="23" spans="1:7" ht="214.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="6"/>
       <c r="D24" s="5">
         <v>4</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="6"/>
-      <c r="B26" s="23" t="s">
+    </row>
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="6" t="s">
+    </row>
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="6" t="s">
+    </row>
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="6" t="s">
+    </row>
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1310,7 +1274,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1318,19 +1282,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="32.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1356,7 +1318,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1382,7 +1344,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1408,7 +1370,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>23</v>
@@ -1419,18 +1381,17 @@
       <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6" t="s">
+      <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>28</v>
@@ -1441,66 +1402,38 @@
       <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="5">
         <v>5</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
archive before cleaning code
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mseduculiegebe-my.sharepoint.com/personal/noe_diffels_student_uliege_be/Documents/Ordi - Bureau/Ordi - ULG/Job - Load Shifting/ULG_Flex_Residential_Load/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_75FB7AE426D7D3644CBF663AB805D8CA4BC093CE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD6AB710-BE7C-49F9-829D-10A633053C7E}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_75FB7AE426D7D3644CBF663AB805D8CA4BC093CE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE5C26B2-76CF-4541-B5EC-F302AFE5EEFA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -602,6 +602,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -895,7 +899,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -953,7 +957,7 @@
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="14">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
EV improvements + title load profile
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
   <si>
     <t>True/False</t>
   </si>
@@ -405,34 +405,19 @@
     <t>[large, medium, small]</t>
   </si>
   <si>
-    <t>EV_statut</t>
-  </si>
-  <si>
-    <t>Statut social de l'utilisateur</t>
-  </si>
-  <si>
-    <t>[working, student, inactive]</t>
-  </si>
-  <si>
-    <t>EV_nb_drivers</t>
-  </si>
-  <si>
-    <t>Nombre de conducteur de EV</t>
-  </si>
-  <si>
-    <t>Pour cette simulation, vaut 1.</t>
-  </si>
-  <si>
     <t>EV_charger_power</t>
   </si>
   <si>
-    <t>Puissance de charge du chargeur</t>
+    <t>Puissance de charge du chargeur [kW]</t>
   </si>
   <si>
     <t>EV_usage</t>
   </si>
   <si>
     <t>Type d'usage du véhicule</t>
+  </si>
+  <si>
+    <t>[short, normal, long, int: (km/year)]</t>
   </si>
   <si>
     <t>Plot</t>
@@ -449,7 +434,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,12 +473,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -568,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -642,17 +621,11 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -962,7 +935,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -971,7 +944,7 @@
     <col min="1" max="1" style="8" width="31.433571428571426" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="8" width="40.57642857142857" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="30" width="27.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="28" width="27.433571428571426" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="8" width="15.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="8" width="2.5764285714285715" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="8" width="56.43357142857143" customWidth="1" bestFit="1"/>
@@ -1074,7 +1047,7 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1289,7 +1262,7 @@
         <v>86</v>
       </c>
       <c r="C21" s="17"/>
-      <c r="D21" s="25">
+      <c r="D21" s="23">
         <v>60</v>
       </c>
       <c r="E21" s="3"/>
@@ -1324,7 +1297,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="5"/>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="25" t="s">
         <v>90</v>
       </c>
       <c r="C24" s="5"/>
@@ -1333,7 +1306,7 @@
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="214.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="208.5">
       <c r="A25" s="3" t="s">
         <v>91</v>
       </c>
@@ -1346,11 +1319,11 @@
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="26" t="s">
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3" t="s">
         <v>94</v>
       </c>
@@ -1376,7 +1349,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="5"/>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="25" t="s">
         <v>96</v>
       </c>
       <c r="C28" s="5"/>
@@ -1394,7 +1367,7 @@
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="4">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -1425,96 +1398,64 @@
         <v>103</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="4" t="s">
-        <v>17</v>
+      <c r="D31" s="6">
+        <v>4</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="5" t="s">
-        <v>104</v>
-      </c>
+      <c r="G31" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="6">
-        <v>1</v>
+      <c r="D32" s="4">
+        <v>100000</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>109</v>
-      </c>
+        <v>106</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="6">
-        <v>4</v>
-      </c>
+      <c r="D33" s="21"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>111</v>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+      <c r="A34" s="5"/>
+      <c r="B34" s="27" t="s">
+        <v>107</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="28">
-        <v>100000</v>
-      </c>
+      <c r="D34" s="21"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+      <c r="A35" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>109</v>
+      </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="21"/>
+      <c r="D35" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
-      <c r="A36" s="5"/>
-      <c r="B36" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
EV usage/size probabilities implementation
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="115">
   <si>
     <t>True/False</t>
   </si>
@@ -399,25 +399,40 @@
     <t>EV_size</t>
   </si>
   <si>
-    <t>Taille du véhicule</t>
-  </si>
-  <si>
-    <t>[large, medium, small]</t>
+    <t>Probabilités de taille du véhicule</t>
+  </si>
+  <si>
+    <t>0.3, 0.5, 0.2</t>
+  </si>
+  <si>
+    <t>[small, medium, large]</t>
+  </si>
+  <si>
+    <t>EV_usage</t>
+  </si>
+  <si>
+    <t>Probabilités de type d'usage du véhicule</t>
+  </si>
+  <si>
+    <t>0.2, 0.5, 0.3</t>
+  </si>
+  <si>
+    <t>[short, normal, long, int: (km/year)]</t>
+  </si>
+  <si>
+    <t>EV_km_per_year</t>
+  </si>
+  <si>
+    <t>Nombre de kilomètres par an (à la place de EV_usage)</t>
+  </si>
+  <si>
+    <t>Si &lt;=0, ne prend pas en compte cet input, simulation en fonciton de EV_usage</t>
   </si>
   <si>
     <t>EV_charger_power</t>
   </si>
   <si>
     <t>Puissance de charge du chargeur [kW]</t>
-  </si>
-  <si>
-    <t>EV_usage</t>
-  </si>
-  <si>
-    <t>Type d'usage du véhicule</t>
-  </si>
-  <si>
-    <t>[short, normal, long, int: (km/year)]</t>
   </si>
   <si>
     <t>Plot</t>
@@ -935,19 +950,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="8" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="40.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="45.29071428571429" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="28" width="27.433571428571426" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="8" width="15.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="8" width="2.5764285714285715" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="56.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="63.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.25">
@@ -1047,7 +1062,7 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="18">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1306,7 +1321,7 @@
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="208.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="195">
       <c r="A25" s="3" t="s">
         <v>91</v>
       </c>
@@ -1382,60 +1397,66 @@
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="4" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="6">
-        <v>4</v>
+      <c r="D31" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="G31" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="4">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+      <c r="A33" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>111</v>
+      </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="21"/>
+      <c r="D33" s="6">
+        <v>4</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="5"/>
-      <c r="B34" s="27" t="s">
-        <v>107</v>
-      </c>
+      <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="21"/>
       <c r="E34" s="5"/>
@@ -1443,19 +1464,48 @@
       <c r="G34" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>109</v>
-      </c>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="D35" s="4"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+      <c r="A37" s="5"/>
+      <c r="B37" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+      <c r="A38" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
improvement EV_daily and new print main
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1074,7 +1074,7 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="18">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="4">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>

</xml_diff>

<commit_message>
implementation simulate(.json) and clean EV
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mseduculiegebe-my.sharepoint.com/personal/noe_diffels_student_uliege_be/Documents/Ordi - Bureau/Ordi - ULG/Job - Load Shifting/ULG_Flex_Residential_Load/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_62EF7ED070D7D374470D808CE3535A08773EE117" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49904538-2C51-45B1-BCB8-6160EA83333E}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="main"/>
-    <sheet r:id="rId2" sheetId="2" name="Liste_données"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="Liste_données" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="123">
   <si>
     <t>True/False</t>
   </si>
@@ -200,6 +206,12 @@
     <t>BE</t>
   </si>
   <si>
+    <t>sim_year</t>
+  </si>
+  <si>
+    <t>Année de la simulation</t>
+  </si>
+  <si>
     <t>Caractéristiques du ménage</t>
   </si>
   <si>
@@ -296,9 +308,6 @@
     <t xml:space="preserve">Type de flexibilité </t>
   </si>
   <si>
-    <r>
-      <t/>
-    </r>
     <r>
       <rPr>
         <b/>
@@ -449,13 +458,24 @@
   <si>
     <t>Make a interactive plot</t>
   </si>
+  <si>
+    <t>0.65</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,12 +493,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -511,6 +525,19 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -521,22 +548,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5983b0"/>
+        <fgColor rgb="FF5983B0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFb2b2b2"/>
+        <fgColor rgb="FFB2B2B2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFf2f2f2"/>
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -557,16 +584,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -574,101 +601,95 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="26">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -679,10 +700,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -720,71 +741,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -812,7 +833,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -835,11 +856,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -848,13 +869,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -864,7 +885,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -873,7 +894,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -882,7 +903,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -890,10 +911,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -958,568 +979,503 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="8" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="45.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="28" width="27.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="2.5764285714285715" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="63.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18">
-        <v>30</v>
-      </c>
-      <c r="E4" s="19" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="16">
+        <v>2</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>48</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="20">
+      <c r="C5" s="14"/>
+      <c r="D5" s="18">
         <v>10</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="17" t="s">
         <v>52</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18">
+      <c r="C6" s="14"/>
+      <c r="D6" s="16">
         <v>2</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18">
-        <v>10</v>
+      <c r="C7" s="14"/>
+      <c r="D7" s="16">
+        <v>1</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="16" t="s">
         <v>60</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="3"/>
-      <c r="B10" s="22" t="s">
+    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="B9" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="25">
+        <v>2024</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="19" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="23">
+      <c r="B12" s="14" t="s">
         <v>1</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="19"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="G12" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="23">
-        <v>4</v>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15">
+        <v>1</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="19"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="24" t="s">
-        <v>22</v>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15">
+        <v>4</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="3" t="s">
+      <c r="B15" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="24" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="16" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="G15" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="24" t="s">
+      <c r="C16" s="14"/>
+      <c r="D16" s="16" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="G16" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="24" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="16" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="G17" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="24" t="s">
-        <v>13</v>
+      <c r="C18" s="14"/>
+      <c r="D18" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="G18" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="24">
-        <v>65</v>
+      <c r="C19" s="14"/>
+      <c r="D19" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="3" t="s">
+      <c r="B20" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="24">
-        <v>60</v>
+      <c r="C20" s="14"/>
+      <c r="D20" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="23">
-        <v>60</v>
+      <c r="C21" s="14"/>
+      <c r="D21" s="18" t="s">
+        <v>120</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="3" t="s">
+      <c r="B22" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="24">
-        <v>25</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="5"/>
-      <c r="B24" s="25" t="s">
+    </row>
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="195">
-      <c r="A25" s="3" t="s">
+      <c r="B23" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="D23" s="18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="15"/>
+    </row>
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="15"/>
+    </row>
+    <row r="26" spans="1:7" ht="195" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="17" t="s">
+      <c r="G26" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6">
+    </row>
+    <row r="27" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="15">
         <v>4</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="5"/>
-      <c r="B28" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="5" t="s">
+    </row>
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D28" s="15"/>
+    </row>
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="4">
+      <c r="D29" s="15"/>
+    </row>
+    <row r="30" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" t="s">
         <v>100</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5" t="s">
+      <c r="B31" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="5" t="s">
+      <c r="D31" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="G31" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="4" t="s">
+    </row>
+    <row r="32" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5" t="s">
+      <c r="B32" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="5" t="s">
+      <c r="D32" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="G32" t="s">
         <v>108</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="4">
+    </row>
+    <row r="33" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="15">
         <v>0</v>
       </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B33" s="5" t="s">
+      <c r="G33" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6" t="s">
+    </row>
+    <row r="34" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5" t="s">
+      <c r="B34" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="5"/>
-      <c r="B37" s="27" t="s">
+      <c r="D34" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
-      <c r="A38" s="5" t="s">
+      <c r="G34" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="5" t="s">
+    </row>
+    <row r="35" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D35" s="15"/>
+    </row>
+    <row r="36" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="15"/>
+    </row>
+    <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D37" s="15"/>
+    </row>
+    <row r="38" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="15"/>
+    </row>
+    <row r="39" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1527,7 +1483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1535,22 +1491,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="23.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="32.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1585,7 +1536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1616,9 +1567,8 @@
       <c r="J2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    </row>
+    <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1628,7 +1578,7 @@
       <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1649,9 +1599,8 @@
       <c r="J3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    </row>
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>28</v>
@@ -1659,26 +1608,23 @@
       <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
+      <c r="G4" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5" t="s">
+      <c r="J4" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    </row>
+    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>34</v>
@@ -1686,84 +1632,43 @@
       <c r="C5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>5</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
washing machine and EV adjust
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -460,7 +460,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -574,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -647,6 +649,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -965,7 +970,7 @@
     <col min="1" max="1" style="7" width="31.433571428571426" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="7" width="45.29071428571429" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="26" width="27.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="27" width="27.433571428571426" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="7" width="15.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="7" width="2.5764285714285715" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="7" width="63.86214285714286" customWidth="1" bestFit="1"/>
@@ -1068,7 +1073,7 @@
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="18">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1265,7 +1270,7 @@
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="20">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1273,7 +1278,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3" t="s">
         <v>84</v>
       </c>
@@ -1282,7 +1287,7 @@
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="20">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1290,7 +1295,7 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3" t="s">
         <v>87</v>
       </c>
@@ -1299,7 +1304,7 @@
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="22">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1307,7 +1312,7 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3" t="s">
         <v>90</v>
       </c>
@@ -1316,13 +1321,13 @@
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="20">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1331,7 +1336,7 @@
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="5"/>
       <c r="B25" s="23" t="s">
         <v>92</v>
@@ -1402,7 +1407,7 @@
         <v>100</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="17">
+      <c r="D30" s="25">
         <v>0.4</v>
       </c>
       <c r="E30" s="5"/>
@@ -1506,7 +1511,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="5"/>
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="26" t="s">
         <v>116</v>
       </c>
       <c r="C38" s="5"/>

</xml_diff>